<commit_message>
Update test usecase excel
</commit_message>
<xml_diff>
--- a/管理端系统测试计划模板.xlsx
+++ b/管理端系统测试计划模板.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="76">
   <si>
     <t>预置条件</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -209,10 +209,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>弹出信息升级成功</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>删除用户</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -221,10 +217,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>弹出信息删除成功</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>选择正确日期</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -258,6 +250,86 @@
   </si>
   <si>
     <t>弹出审核通过信息</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>搜索场馆</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>输入正确的数据类型</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加场馆</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>输入正确的数据格式</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>编辑场馆</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>弹出添加成功/失败信息</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>弹出编辑成功/失败信息</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加新闻</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除新闻</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>选择新闻不为空</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>弹出升级成功/失败信息</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>弹出删除成功/失败信息</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>编辑新闻</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>是</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看图片</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>新闻存在图片</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>弹出显示图片的对话框</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>搜索留言</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>审核通过留言</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>留言存在且未通过</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -934,7 +1006,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4272,8 +4344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
@@ -4467,7 +4539,7 @@
         <v>40</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
@@ -4493,7 +4565,7 @@
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>26</v>
@@ -4508,14 +4580,14 @@
         <v>4</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>26</v>
@@ -4530,14 +4602,14 @@
         <v>5</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>26</v>
@@ -4552,10 +4624,10 @@
         <v>6</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
@@ -4574,14 +4646,14 @@
         <v>6</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>26</v>
@@ -4592,100 +4664,198 @@
       <c r="A15" s="3">
         <v>13</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+      <c r="B15" s="3">
+        <v>7</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+      <c r="F15" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="G15" s="3" t="s">
         <v>26</v>
       </c>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
+      <c r="A16" s="3">
+        <v>14</v>
+      </c>
+      <c r="B16" s="3">
+        <v>7</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="F16" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="G16" s="3" t="s">
         <v>26</v>
       </c>
       <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
+      <c r="A17" s="3">
+        <v>15</v>
+      </c>
+      <c r="B17" s="3">
+        <v>7</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
+      <c r="F17" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="G17" s="3" t="s">
         <v>26</v>
       </c>
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
+      <c r="A18" s="3">
+        <v>16</v>
+      </c>
+      <c r="B18" s="3">
+        <v>8</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
+      <c r="F18" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="G18" s="3" t="s">
         <v>26</v>
       </c>
       <c r="H18" s="3"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
+      <c r="A19" s="3">
+        <v>17</v>
+      </c>
+      <c r="B19" s="3">
+        <v>8</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>65</v>
+      </c>
       <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
+      <c r="F19" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="H19" s="3"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
+      <c r="A20" s="3">
+        <v>18</v>
+      </c>
+      <c r="B20" s="3">
+        <v>8</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
+      <c r="F20" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>69</v>
+      </c>
       <c r="H20" s="3"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
+      <c r="A21" s="3">
+        <v>19</v>
+      </c>
+      <c r="B21" s="3">
+        <v>8</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
+      <c r="F21" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>69</v>
+      </c>
       <c r="H21" s="3"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
+      <c r="A22" s="3">
+        <v>20</v>
+      </c>
+      <c r="B22" s="3">
+        <v>9</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
+      <c r="F22" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>69</v>
+      </c>
       <c r="H22" s="3"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
+      <c r="A23" s="3">
+        <v>21</v>
+      </c>
+      <c r="B23" s="3">
+        <v>9</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>75</v>
+      </c>
       <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
+      <c r="F23" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>69</v>
+      </c>
       <c r="H23" s="3"/>
     </row>
     <row r="24" spans="1:8">

</xml_diff>